<commit_message>
DF Some fixes in imports.
</commit_message>
<xml_diff>
--- a/mes-plugins/mes-plugins-material-flow-resources/src/main/resources/materialFlowResources/public/resources/positionImportSchema_de.xlsx
+++ b/mes-plugins/mes-plugins-material-flow-resources/src/main/resources/materialFlowResources/public/resources/positionImportSchema_de.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lupo/qcadoo-src/mes/mes-plugins/mes-plugins-material-flow-resources/src/main/resources/materialFlowResources/public/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB85381F-A429-9E45-A702-0D1E725D94D4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97D7E7F4-3EC0-C240-A8D2-3B5174FE66AE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16760" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -400,16 +400,12 @@
   <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="17.6640625" customWidth="1"/>
-    <col min="7" max="8" width="14" customWidth="1"/>
-    <col min="9" max="9" width="14.6640625" customWidth="1"/>
-    <col min="10" max="10" width="12.5" customWidth="1"/>
-    <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
+    <col min="1" max="11" width="16.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">

</xml_diff>